<commit_message>
Adapted Excel Doku to Panel Exam
</commit_message>
<xml_diff>
--- a/Projektdetails_WS24_Komm_canic.xlsx
+++ b/Projektdetails_WS24_Komm_canic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canic\IdeaProjects\ODE2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B36F47D-6E88-433A-97BA-630EBE06225F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05143C20-B67F-420A-9EA6-548AA017470D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -24,24 +24,11 @@
     <sheet name="PPX Beispiel" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t>Informationen</t>
   </si>
@@ -447,12 +434,6 @@
     <t xml:space="preserve">    &lt;Should have feature 2&gt; getestet</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;Should have feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 3&gt; getestet</t>
-  </si>
-  <si>
     <t>Nice to haves</t>
   </si>
   <si>
@@ -466,12 +447,6 @@
   </si>
   <si>
     <t xml:space="preserve">    &lt;Nice to have feature 2&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 3&gt; getestet</t>
   </si>
   <si>
     <t>Overkill</t>
@@ -489,12 +464,6 @@
     <t xml:space="preserve">    &lt;Overkill feature 2&gt; getestet</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;Overkill feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Overkill feature 3&gt; getestet</t>
-  </si>
-  <si>
     <t>Präsentations slot ist eingetragen (moodle)</t>
   </si>
   <si>
@@ -507,37 +476,19 @@
     <t>Titel</t>
   </si>
   <si>
-    <t>&lt;Titel des Projekts&gt;</t>
-  </si>
-  <si>
     <t>Beschreibung</t>
-  </si>
-  <si>
-    <t>&lt;Kurze Beschreibung, kann auch Vergleiche mit bestehenden Applikationen beinhalten (zB Slack ähnliche Chat Applikation)&gt;</t>
   </si>
   <si>
     <t>Team</t>
   </si>
   <si>
-    <t>&lt;Name inkl. git name und Personenkennzeichen&gt;</t>
-  </si>
-  <si>
     <t>Link zum Repo</t>
-  </si>
-  <si>
-    <t>&lt;Link zum public git repo, private repo mit invite oder FH git repo&gt;</t>
   </si>
   <si>
     <t>Link zum Board</t>
   </si>
   <si>
-    <t>&lt;Link zum Board mit Tickets zB Trello, git&gt;</t>
-  </si>
-  <si>
     <t>Must have features (genügend)</t>
-  </si>
-  <si>
-    <t>&lt;Listen Sie die jeweiligen Features mind. eines pro Person und Kategorie&gt;</t>
   </si>
   <si>
     <t>Should have features (befriedigend)</t>
@@ -775,12 +726,39 @@
       <t>(müssen alle erfüllt sein um von "gut" auf "sehr gut" zu kommen)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">    &lt;Must have feature 4&gt; erledigt und gemerged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;Must have feature 4&gt; getestet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;Must have feature 5&gt; erledigt und gemerged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;Must have feature 5&gt; getestet</t>
+  </si>
+  <si>
+    <t>ODE 2025 (TicTacToe Canic)</t>
+  </si>
+  <si>
+    <t>TicTacToe game, PvP over network, Overkill PvPC (AI)</t>
+  </si>
+  <si>
+    <t>Canic (anastasija2004)</t>
+  </si>
+  <si>
+    <t>https://github.com/anastasija2004/ODE2025</t>
+  </si>
+  <si>
+    <t>https://github.com/users/anastasija2004/projects/1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -854,6 +832,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -881,10 +866,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -923,8 +909,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1143,7 +1133,7 @@
   </sheetPr>
   <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1188,10 +1178,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:C1050"/>
+  <dimension ref="B1:C1048"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1370,155 +1360,149 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="12.5">
+    <row r="29" spans="2:3" ht="12" customHeight="1">
       <c r="B29" s="3"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="12.5">
-      <c r="B30" s="5"/>
-      <c r="C30" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="12.5">
+    <row r="30" spans="2:3" ht="12" customHeight="1">
+      <c r="B30" s="3"/>
+      <c r="C30" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="12" customHeight="1">
       <c r="B31" s="3"/>
       <c r="C31" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="12.5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="12" customHeight="1">
       <c r="B32" s="3"/>
       <c r="C32" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="12.5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="12" customHeight="1">
       <c r="B33" s="3"/>
       <c r="C33" s="7" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="12.5">
-      <c r="B34" s="3"/>
-      <c r="C34" s="7" t="s">
-        <v>38</v>
+      <c r="B34" s="5"/>
+      <c r="C34" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="12.5">
       <c r="B35" s="3"/>
       <c r="C35" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="12.5">
       <c r="B36" s="3"/>
       <c r="C36" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="12.5">
-      <c r="B37" s="5"/>
-      <c r="C37" s="8" t="s">
-        <v>41</v>
+      <c r="B37" s="3"/>
+      <c r="C37" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="12.5">
       <c r="B38" s="3"/>
       <c r="C38" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="12.5">
-      <c r="B39" s="3"/>
-      <c r="C39" s="7" t="s">
-        <v>43</v>
+      <c r="B39" s="5"/>
+      <c r="C39" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="12.5">
       <c r="B40" s="3"/>
       <c r="C40" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="12.5">
       <c r="B41" s="3"/>
       <c r="C41" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="12.5">
       <c r="B42" s="3"/>
       <c r="C42" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="12.5">
       <c r="B43" s="3"/>
       <c r="C43" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="12.5">
       <c r="B44" s="5"/>
       <c r="C44" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="12.5">
       <c r="B45" s="3"/>
       <c r="C45" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="12.5">
       <c r="B46" s="3"/>
       <c r="C46" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="12.5">
       <c r="B47" s="3"/>
       <c r="C47" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="12.5">
       <c r="B48" s="3"/>
       <c r="C48" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="12.5">
-      <c r="B49" s="3"/>
-      <c r="C49" s="7" t="s">
-        <v>53</v>
+      <c r="B49" s="5"/>
+      <c r="C49" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="12.5">
       <c r="B50" s="3"/>
       <c r="C50" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="12.5">
-      <c r="B51" s="5"/>
-      <c r="C51" s="8" t="s">
-        <v>55</v>
+      <c r="B51" s="3"/>
+      <c r="C51" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="12.5">
       <c r="B52" s="3"/>
-      <c r="C52" s="7" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="53" spans="2:3" ht="12.5">
       <c r="B53" s="3"/>
-      <c r="C53" s="7" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="54" spans="2:3" ht="12.5">
       <c r="B54" s="3"/>
@@ -4504,12 +4488,6 @@
     </row>
     <row r="1048" spans="2:2" ht="12.5">
       <c r="B1048" s="3"/>
-    </row>
-    <row r="1049" spans="2:2" ht="12.5">
-      <c r="B1049" s="3"/>
-    </row>
-    <row r="1050" spans="2:2" ht="12.5">
-      <c r="B1050" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4523,8 +4501,8 @@
   </sheetPr>
   <dimension ref="B1:C1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -4540,54 +4518,50 @@
     </row>
     <row r="2" spans="2:3" ht="13">
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="61.5" customHeight="1">
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="12.5">
       <c r="B4" s="15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12.5">
       <c r="B5" s="16"/>
-      <c r="C5" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:3" ht="12.5">
       <c r="B6" s="16"/>
-      <c r="C6" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="2:3" ht="26">
       <c r="B7" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="26">
       <c r="B8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="13">
@@ -4596,11 +4570,9 @@
     </row>
     <row r="10" spans="2:3" ht="12.5">
       <c r="B10" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>69</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="2:3" ht="12.5">
       <c r="B11" s="16"/>
@@ -4616,7 +4588,7 @@
     </row>
     <row r="14" spans="2:3" ht="12.5">
       <c r="B14" s="15" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C14" s="10"/>
     </row>
@@ -4634,7 +4606,7 @@
     </row>
     <row r="18" spans="2:3" ht="12.5">
       <c r="B18" s="15" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C18" s="10"/>
     </row>
@@ -4652,7 +4624,7 @@
     </row>
     <row r="22" spans="2:3" ht="12.5">
       <c r="B22" s="15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C22" s="10"/>
     </row>
@@ -8580,6 +8552,10 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{102953C7-7871-46EE-8609-D51B78842DB3}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{C094C9E5-7FF2-4BFA-BE3F-6C9F94C7B04F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8591,7 +8567,7 @@
   </sheetPr>
   <dimension ref="B2:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -8604,22 +8580,22 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8647,22 +8623,22 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8690,22 +8666,22 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8733,22 +8709,22 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8780,54 +8756,54 @@
     </row>
     <row r="2" spans="2:3" ht="13">
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="61.5" customHeight="1">
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="12.5">
       <c r="B4" s="15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12.5">
       <c r="B5" s="16"/>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="12.5">
       <c r="B6" s="16"/>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="13">
       <c r="B7" s="9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="13">
       <c r="B8" s="9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="13">
@@ -8836,22 +8812,22 @@
     </row>
     <row r="10" spans="2:3" ht="12.5">
       <c r="B10" s="17" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="12.5">
       <c r="B11" s="16"/>
       <c r="C11" s="10" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="12.5">
       <c r="B12" s="16"/>
       <c r="C12" s="10" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="12.5">
@@ -8860,22 +8836,22 @@
     </row>
     <row r="14" spans="2:3" ht="12.5">
       <c r="B14" s="17" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="12.5">
       <c r="B15" s="16"/>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12.5">
       <c r="B16" s="16"/>
       <c r="C16" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1">
@@ -8883,22 +8859,22 @@
     </row>
     <row r="18" spans="2:3" ht="12.5">
       <c r="B18" s="17" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="12.5">
       <c r="B19" s="16"/>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="12.5">
       <c r="B20" s="16"/>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
@@ -8906,22 +8882,22 @@
     </row>
     <row r="22" spans="2:3" ht="12.5">
       <c r="B22" s="17" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="12.5">
       <c r="B23" s="16"/>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="12.5">
       <c r="B24" s="16"/>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
@@ -12866,185 +12842,185 @@
     <col min="7" max="7" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" ht="13">
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E3" s="2">
         <v>1.5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2">
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2">
         <v>0.25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" customHeight="1">
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2">
         <v>1.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1">
       <c r="B12" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>